<commit_message>
Correction of  minor errors and added simplifications
Correct minor errors and added some simplifications
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hans Verkerk\Desktop\GIT\SwitchInterfaceParser\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAFE5CA-7829-4803-9DA4-6802D20D9B9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Portinfo" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Vlaninfo" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Portinfo" sheetId="1" r:id="rId1"/>
+    <sheet name="Vlaninfo" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
   <si>
     <t>hostname</t>
   </si>
@@ -295,20 +300,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -324,15 +328,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -620,20 +633,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection sqref="A1:U1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -695,7 +726,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -705,33 +736,20 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s"/>
-      <c r="E2" t="s"/>
-      <c r="F2" t="s"/>
-      <c r="G2" t="s"/>
-      <c r="H2" t="s"/>
-      <c r="I2" t="s"/>
-      <c r="J2" t="s"/>
-      <c r="K2" t="s"/>
-      <c r="L2" t="s"/>
       <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s"/>
-      <c r="O2" t="s"/>
       <c r="P2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" t="s"/>
       <c r="R2" t="s">
         <v>23</v>
       </c>
       <c r="S2" t="s">
         <v>25</v>
       </c>
-      <c r="T2" t="s"/>
-    </row>
-    <row r="3" spans="1:20">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -741,33 +759,20 @@
       <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s"/>
-      <c r="E3" t="s"/>
-      <c r="F3" t="s"/>
-      <c r="G3" t="s"/>
-      <c r="H3" t="s"/>
-      <c r="I3" t="s"/>
       <c r="J3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" t="s"/>
-      <c r="L3" t="s"/>
       <c r="M3" t="s">
         <v>12</v>
       </c>
-      <c r="N3" t="s"/>
-      <c r="O3" t="s"/>
-      <c r="P3" t="s"/>
       <c r="Q3" t="s">
         <v>29</v>
       </c>
       <c r="R3" t="s">
         <v>30</v>
       </c>
-      <c r="S3" t="s"/>
-      <c r="T3" t="s"/>
-    </row>
-    <row r="4" spans="1:20">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -777,33 +782,20 @@
       <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s"/>
-      <c r="E4" t="s"/>
-      <c r="F4" t="s"/>
-      <c r="G4" t="s"/>
-      <c r="H4" t="s"/>
-      <c r="I4" t="s"/>
       <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="K4" t="s"/>
       <c r="L4" t="s">
         <v>33</v>
       </c>
-      <c r="M4" t="s"/>
-      <c r="N4" t="s"/>
-      <c r="O4" t="s"/>
-      <c r="P4" t="s"/>
       <c r="Q4" t="s">
         <v>34</v>
       </c>
       <c r="R4" t="s">
         <v>30</v>
       </c>
-      <c r="S4" t="s"/>
-      <c r="T4" t="s"/>
-    </row>
-    <row r="5" spans="1:20">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -813,17 +805,9 @@
       <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s"/>
-      <c r="E5" t="s"/>
-      <c r="F5" t="s"/>
-      <c r="G5" t="s"/>
-      <c r="H5" t="s"/>
-      <c r="I5" t="s"/>
       <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="K5" t="s"/>
-      <c r="L5" t="s"/>
       <c r="M5" t="s">
         <v>12</v>
       </c>
@@ -833,25 +817,17 @@
       <c r="O5" t="s">
         <v>38</v>
       </c>
-      <c r="P5" t="s"/>
       <c r="Q5" t="s">
         <v>39</v>
       </c>
-      <c r="R5" t="s"/>
-      <c r="S5" t="s"/>
-      <c r="T5" t="s"/>
-    </row>
-    <row r="6" spans="1:20">
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s"/>
-      <c r="D6" t="s"/>
-      <c r="E6" t="s"/>
-      <c r="F6" t="s"/>
       <c r="G6" t="s">
         <v>41</v>
       </c>
@@ -861,21 +837,11 @@
       <c r="I6" t="s">
         <v>43</v>
       </c>
-      <c r="J6" t="s"/>
-      <c r="K6" t="s"/>
-      <c r="L6" t="s"/>
-      <c r="M6" t="s"/>
-      <c r="N6" t="s"/>
-      <c r="O6" t="s"/>
-      <c r="P6" t="s"/>
-      <c r="Q6" t="s"/>
-      <c r="R6" t="s"/>
-      <c r="S6" t="s"/>
       <c r="T6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -885,35 +851,23 @@
       <c r="C7" t="s">
         <v>46</v>
       </c>
-      <c r="D7" t="s"/>
-      <c r="E7" t="s"/>
       <c r="F7" t="s">
         <v>47</v>
       </c>
-      <c r="G7" t="s"/>
-      <c r="H7" t="s"/>
-      <c r="I7" t="s"/>
-      <c r="J7" t="s"/>
-      <c r="K7" t="s"/>
-      <c r="L7" t="s"/>
-      <c r="M7" t="s"/>
       <c r="N7" t="s">
         <v>37</v>
       </c>
       <c r="O7" t="s">
         <v>48</v>
       </c>
-      <c r="P7" t="s"/>
       <c r="Q7" t="s">
         <v>29</v>
       </c>
       <c r="R7" t="s">
         <v>30</v>
       </c>
-      <c r="S7" t="s"/>
-      <c r="T7" t="s"/>
-    </row>
-    <row r="8" spans="1:20">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -923,35 +877,23 @@
       <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" t="s"/>
-      <c r="E8" t="s"/>
       <c r="F8" t="s">
         <v>51</v>
       </c>
-      <c r="G8" t="s"/>
-      <c r="H8" t="s"/>
-      <c r="I8" t="s"/>
-      <c r="J8" t="s"/>
-      <c r="K8" t="s"/>
-      <c r="L8" t="s"/>
-      <c r="M8" t="s"/>
       <c r="N8" t="s">
         <v>37</v>
       </c>
       <c r="O8" t="s">
         <v>48</v>
       </c>
-      <c r="P8" t="s"/>
       <c r="Q8" t="s">
         <v>34</v>
       </c>
       <c r="R8" t="s">
         <v>30</v>
       </c>
-      <c r="S8" t="s"/>
-      <c r="T8" t="s"/>
-    </row>
-    <row r="9" spans="1:20">
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -961,17 +903,9 @@
       <c r="C9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" t="s"/>
-      <c r="E9" t="s"/>
       <c r="F9" t="s">
         <v>54</v>
       </c>
-      <c r="G9" t="s"/>
-      <c r="H9" t="s"/>
-      <c r="I9" t="s"/>
-      <c r="J9" t="s"/>
-      <c r="K9" t="s"/>
-      <c r="L9" t="s"/>
       <c r="M9" t="s">
         <v>23</v>
       </c>
@@ -981,17 +915,14 @@
       <c r="O9" t="s">
         <v>48</v>
       </c>
-      <c r="P9" t="s"/>
       <c r="Q9" t="s">
         <v>39</v>
       </c>
       <c r="R9" t="s">
         <v>30</v>
       </c>
-      <c r="S9" t="s"/>
-      <c r="T9" t="s"/>
-    </row>
-    <row r="10" spans="1:20">
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1001,20 +932,9 @@
       <c r="C10" t="s">
         <v>56</v>
       </c>
-      <c r="D10" t="s"/>
       <c r="E10" t="s">
         <v>57</v>
       </c>
-      <c r="F10" t="s"/>
-      <c r="G10" t="s"/>
-      <c r="H10" t="s"/>
-      <c r="I10" t="s"/>
-      <c r="J10" t="s"/>
-      <c r="K10" t="s"/>
-      <c r="L10" t="s"/>
-      <c r="M10" t="s"/>
-      <c r="N10" t="s"/>
-      <c r="O10" t="s"/>
       <c r="P10" t="s">
         <v>24</v>
       </c>
@@ -1024,10 +944,8 @@
       <c r="R10" t="s">
         <v>30</v>
       </c>
-      <c r="S10" t="s"/>
-      <c r="T10" t="s"/>
-    </row>
-    <row r="11" spans="1:20">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1037,87 +955,39 @@
       <c r="C11" t="s">
         <v>59</v>
       </c>
-      <c r="D11" t="s"/>
-      <c r="E11" t="s"/>
-      <c r="F11" t="s"/>
-      <c r="G11" t="s"/>
-      <c r="H11" t="s"/>
-      <c r="I11" t="s"/>
-      <c r="J11" t="s"/>
-      <c r="K11" t="s"/>
-      <c r="L11" t="s"/>
       <c r="M11" t="s">
         <v>12</v>
       </c>
-      <c r="N11" t="s"/>
-      <c r="O11" t="s"/>
-      <c r="P11" t="s"/>
       <c r="Q11" t="s">
         <v>39</v>
       </c>
       <c r="R11" t="s">
         <v>30</v>
       </c>
-      <c r="S11" t="s"/>
-      <c r="T11" t="s"/>
-    </row>
-    <row r="12" spans="1:20">
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>60</v>
       </c>
-      <c r="C12" t="s"/>
-      <c r="D12" t="s"/>
-      <c r="E12" t="s"/>
-      <c r="F12" t="s"/>
-      <c r="G12" t="s"/>
-      <c r="H12" t="s"/>
-      <c r="I12" t="s"/>
-      <c r="J12" t="s"/>
       <c r="K12" t="s">
         <v>10</v>
       </c>
-      <c r="L12" t="s"/>
-      <c r="M12" t="s"/>
-      <c r="N12" t="s"/>
-      <c r="O12" t="s"/>
-      <c r="P12" t="s"/>
-      <c r="Q12" t="s"/>
-      <c r="R12" t="s"/>
-      <c r="S12" t="s"/>
-      <c r="T12" t="s"/>
-    </row>
-    <row r="13" spans="1:20">
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" t="s"/>
-      <c r="D13" t="s"/>
-      <c r="E13" t="s"/>
-      <c r="F13" t="s"/>
-      <c r="G13" t="s"/>
-      <c r="H13" t="s"/>
-      <c r="I13" t="s"/>
-      <c r="J13" t="s"/>
       <c r="K13" t="s">
         <v>10</v>
       </c>
-      <c r="L13" t="s"/>
-      <c r="M13" t="s"/>
-      <c r="N13" t="s"/>
-      <c r="O13" t="s"/>
-      <c r="P13" t="s"/>
-      <c r="Q13" t="s"/>
-      <c r="R13" t="s"/>
-      <c r="S13" t="s"/>
-      <c r="T13" t="s"/>
-    </row>
-    <row r="14" spans="1:20">
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1127,115 +997,50 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="D14" t="s"/>
-      <c r="E14" t="s"/>
       <c r="F14" t="s">
         <v>63</v>
       </c>
-      <c r="G14" t="s"/>
-      <c r="H14" t="s"/>
-      <c r="I14" t="s"/>
-      <c r="J14" t="s"/>
-      <c r="K14" t="s"/>
-      <c r="L14" t="s"/>
-      <c r="M14" t="s"/>
-      <c r="N14" t="s"/>
-      <c r="O14" t="s"/>
       <c r="P14" t="s">
         <v>24</v>
       </c>
-      <c r="Q14" t="s"/>
       <c r="R14" t="s">
         <v>23</v>
       </c>
-      <c r="S14" t="s"/>
-      <c r="T14" t="s"/>
-    </row>
-    <row r="15" spans="1:20">
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="C15" t="s"/>
-      <c r="D15" t="s"/>
-      <c r="E15" t="s"/>
-      <c r="F15" t="s"/>
-      <c r="G15" t="s"/>
-      <c r="H15" t="s"/>
-      <c r="I15" t="s"/>
-      <c r="J15" t="s"/>
       <c r="K15" t="s">
         <v>10</v>
       </c>
-      <c r="L15" t="s"/>
-      <c r="M15" t="s"/>
-      <c r="N15" t="s"/>
-      <c r="O15" t="s"/>
-      <c r="P15" t="s"/>
-      <c r="Q15" t="s"/>
-      <c r="R15" t="s"/>
-      <c r="S15" t="s"/>
-      <c r="T15" t="s"/>
-    </row>
-    <row r="16" spans="1:20">
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>65</v>
       </c>
-      <c r="C16" t="s"/>
-      <c r="D16" t="s"/>
-      <c r="E16" t="s"/>
-      <c r="F16" t="s"/>
-      <c r="G16" t="s"/>
-      <c r="H16" t="s"/>
-      <c r="I16" t="s"/>
-      <c r="J16" t="s"/>
       <c r="K16" t="s">
         <v>10</v>
       </c>
-      <c r="L16" t="s"/>
-      <c r="M16" t="s"/>
-      <c r="N16" t="s"/>
-      <c r="O16" t="s"/>
-      <c r="P16" t="s"/>
-      <c r="Q16" t="s"/>
-      <c r="R16" t="s"/>
-      <c r="S16" t="s"/>
-      <c r="T16" t="s"/>
-    </row>
-    <row r="17" spans="1:20">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
         <v>66</v>
       </c>
-      <c r="C17" t="s"/>
-      <c r="D17" t="s"/>
-      <c r="E17" t="s"/>
-      <c r="F17" t="s"/>
-      <c r="G17" t="s"/>
-      <c r="H17" t="s"/>
-      <c r="I17" t="s"/>
-      <c r="J17" t="s"/>
       <c r="K17" t="s">
         <v>10</v>
       </c>
-      <c r="L17" t="s"/>
-      <c r="M17" t="s"/>
-      <c r="N17" t="s"/>
-      <c r="O17" t="s"/>
-      <c r="P17" t="s"/>
-      <c r="Q17" t="s"/>
-      <c r="R17" t="s"/>
-      <c r="S17" t="s"/>
-      <c r="T17" t="s"/>
-    </row>
-    <row r="18" spans="1:20">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1245,35 +1050,23 @@
       <c r="C18" t="s">
         <v>68</v>
       </c>
-      <c r="D18" t="s"/>
-      <c r="E18" t="s"/>
       <c r="F18" t="s">
         <v>47</v>
       </c>
-      <c r="G18" t="s"/>
-      <c r="H18" t="s"/>
-      <c r="I18" t="s"/>
-      <c r="J18" t="s"/>
-      <c r="K18" t="s"/>
-      <c r="L18" t="s"/>
-      <c r="M18" t="s"/>
       <c r="N18" t="s">
         <v>37</v>
       </c>
       <c r="O18" t="s">
         <v>48</v>
       </c>
-      <c r="P18" t="s"/>
       <c r="Q18" t="s">
         <v>29</v>
       </c>
       <c r="R18" t="s">
         <v>30</v>
       </c>
-      <c r="S18" t="s"/>
-      <c r="T18" t="s"/>
-    </row>
-    <row r="19" spans="1:20">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1283,31 +1076,17 @@
       <c r="C19" t="s">
         <v>68</v>
       </c>
-      <c r="D19" t="s"/>
-      <c r="E19" t="s"/>
       <c r="F19" t="s">
         <v>51</v>
       </c>
-      <c r="G19" t="s"/>
-      <c r="H19" t="s"/>
-      <c r="I19" t="s"/>
-      <c r="J19" t="s"/>
-      <c r="K19" t="s"/>
-      <c r="L19" t="s"/>
-      <c r="M19" t="s"/>
-      <c r="N19" t="s"/>
-      <c r="O19" t="s"/>
-      <c r="P19" t="s"/>
       <c r="Q19" t="s">
         <v>34</v>
       </c>
       <c r="R19" t="s">
         <v>30</v>
       </c>
-      <c r="S19" t="s"/>
-      <c r="T19" t="s"/>
-    </row>
-    <row r="20" spans="1:20">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1317,31 +1096,17 @@
       <c r="C20" t="s">
         <v>68</v>
       </c>
-      <c r="D20" t="s"/>
-      <c r="E20" t="s"/>
       <c r="F20" t="s">
         <v>54</v>
       </c>
-      <c r="G20" t="s"/>
-      <c r="H20" t="s"/>
-      <c r="I20" t="s"/>
-      <c r="J20" t="s"/>
-      <c r="K20" t="s"/>
-      <c r="L20" t="s"/>
-      <c r="M20" t="s"/>
-      <c r="N20" t="s"/>
-      <c r="O20" t="s"/>
-      <c r="P20" t="s"/>
       <c r="Q20" t="s">
         <v>39</v>
       </c>
       <c r="R20" t="s">
         <v>30</v>
       </c>
-      <c r="S20" t="s"/>
-      <c r="T20" t="s"/>
-    </row>
-    <row r="21" spans="1:20">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1354,49 +1119,45 @@
       <c r="D21" t="s">
         <v>72</v>
       </c>
-      <c r="E21" t="s"/>
       <c r="F21" t="s">
         <v>63</v>
       </c>
-      <c r="G21" t="s"/>
-      <c r="H21" t="s"/>
-      <c r="I21" t="s"/>
-      <c r="J21" t="s"/>
-      <c r="K21" t="s"/>
-      <c r="L21" t="s"/>
-      <c r="M21" t="s"/>
-      <c r="N21" t="s"/>
-      <c r="O21" t="s"/>
       <c r="P21" t="s">
         <v>24</v>
       </c>
-      <c r="Q21" t="s"/>
       <c r="R21" t="s">
         <v>23</v>
       </c>
-      <c r="S21" t="s"/>
-      <c r="T21" t="s"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1:R1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1431,7 +1192,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1441,7 +1202,6 @@
       <c r="C2" t="s">
         <v>80</v>
       </c>
-      <c r="D2" t="s"/>
       <c r="E2" t="s">
         <v>81</v>
       </c>
@@ -1451,16 +1211,14 @@
       <c r="G2" t="s">
         <v>83</v>
       </c>
-      <c r="H2" t="s"/>
       <c r="I2" t="s">
         <v>42</v>
       </c>
-      <c r="J2" t="s"/>
       <c r="K2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1476,16 +1234,11 @@
       <c r="E3" t="s">
         <v>81</v>
       </c>
-      <c r="F3" t="s"/>
-      <c r="G3" t="s"/>
       <c r="H3" t="s">
         <v>87</v>
       </c>
-      <c r="I3" t="s"/>
-      <c r="J3" t="s"/>
-      <c r="K3" t="s"/>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1495,16 +1248,8 @@
       <c r="C4" t="s">
         <v>88</v>
       </c>
-      <c r="D4" t="s"/>
-      <c r="E4" t="s"/>
-      <c r="F4" t="s"/>
-      <c r="G4" t="s"/>
-      <c r="H4" t="s"/>
-      <c r="I4" t="s"/>
-      <c r="J4" t="s"/>
-      <c r="K4" t="s"/>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1514,57 +1259,37 @@
       <c r="C5" t="s">
         <v>90</v>
       </c>
-      <c r="D5" t="s"/>
-      <c r="E5" t="s"/>
-      <c r="F5" t="s"/>
-      <c r="G5" t="s"/>
-      <c r="H5" t="s"/>
-      <c r="I5" t="s"/>
-      <c r="J5" t="s"/>
-      <c r="K5" t="s"/>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s"/>
-      <c r="D6" t="s"/>
       <c r="E6" t="s">
         <v>41</v>
       </c>
-      <c r="F6" t="s"/>
-      <c r="G6" t="s"/>
-      <c r="H6" t="s"/>
       <c r="I6" t="s">
         <v>42</v>
       </c>
       <c r="J6" t="s">
         <v>10</v>
       </c>
-      <c r="K6" t="s"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>